<commit_message>
Alterações dashboard geral e especifica
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Product Backlog & Gráfico de Burndown - BeeTech.xlsx
+++ b/Tecnologia da Informação/Product Backlog & Gráfico de Burndown - BeeTech.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\beetech\Sprint_2\Tecnologia da Informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E9AC96-3D7C-439B-B77A-791433CBD60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB588CCD-5F0B-4B9D-9529-2FDE958E84DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F13FE21-3909-4024-9E51-F6B5B91CD81C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="132">
   <si>
     <t>PRODUCT BACKLOG - BEETECH</t>
   </si>
@@ -432,13 +433,16 @@
   </si>
   <si>
     <t>planejado</t>
+  </si>
+  <si>
+    <t>Sprint4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +480,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -491,7 +502,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -588,11 +599,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,13 +643,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -640,11 +663,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,9 +1004,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$K$22:$K$25</c:f>
+              <c:f>Planilha1!$K$22:$K$26</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>total</c:v>
                 </c:pt>
@@ -990,25 +1019,31 @@
                 <c:pt idx="3">
                   <c:v>Sprint3</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint4</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$M$22:$M$25</c:f>
+              <c:f>Planilha1!$M$22:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>286.66666666666663</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>143.33333333333337</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1049,9 +1084,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$K$22:$K$25</c:f>
+              <c:f>Planilha1!$K$22:$K$26</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>total</c:v>
                 </c:pt>
@@ -1064,17 +1099,20 @@
                 <c:pt idx="3">
                   <c:v>Sprint3</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint4</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$N$22:$N$25</c:f>
+              <c:f>Planilha1!$N$22:$N$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>349</c:v>
+                  <c:v>430</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>173</c:v>
@@ -1083,7 +1121,7 @@
                   <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1908,15 +1946,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>344915</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>312088</xdr:rowOff>
+      <xdr:colOff>141715</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>58088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>236482</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>118240</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2285,8 +2323,8 @@
   </sheetPr>
   <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="65" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2312,16 +2350,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2834,13 +2872,13 @@
       <c r="H20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
     </row>
     <row r="21" spans="1:16" ht="30" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -2855,7 +2893,7 @@
       <c r="D21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2868,22 +2906,22 @@
       <c r="H21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="N21" s="11" t="s">
+      <c r="N21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="O21" s="11" t="s">
+      <c r="O21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="17"/>
+      <c r="P21" s="19"/>
     </row>
     <row r="22" spans="1:16" ht="30" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -2898,7 +2936,7 @@
       <c r="D22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2911,24 +2949,24 @@
       <c r="H22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="L22" s="11">
-        <f>SUM(Tabela1[TAM('#)])</f>
+      <c r="L22" s="18">
+        <f>SUM(L23:L26)</f>
         <v>430</v>
       </c>
-      <c r="M22" s="11">
-        <f>SUM(Tabela1[TAM('#)])</f>
+      <c r="M22" s="18">
+        <f>SUM(M23:M26)</f>
         <v>430</v>
       </c>
-      <c r="N22" s="11">
-        <f>SUMIF(Tabela1[ESTADO],"FINALIZADO",Tabela1[TAM('#)])</f>
-        <v>349</v>
-      </c>
-      <c r="O22" s="11">
+      <c r="N22" s="18">
+        <f>SUM(N23:N26)</f>
+        <v>430</v>
+      </c>
+      <c r="O22" s="13">
         <f>SUM(L22-N22)</f>
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="30" customHeight="1">
@@ -2944,7 +2982,7 @@
       <c r="D23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -2957,22 +2995,21 @@
       <c r="H23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="13">
         <f>SUMIF(Tabela1[SPRINT],"SPRINT1",Tabela1[TAM('#)])</f>
         <v>173</v>
       </c>
-      <c r="M23" s="11">
-        <f>M22-(M22/3)</f>
-        <v>286.66666666666663</v>
-      </c>
-      <c r="N23" s="12">
+      <c r="M23" s="13">
+        <v>165</v>
+      </c>
+      <c r="N23" s="11">
         <f>SUMIFS(Tabela1[TAM('#)],Tabela1[ESTADO],"FINALIZADO",Tabela1[SPRINT],"SPRINT1")</f>
         <v>173</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="13">
         <f>SUM(L23-N23)</f>
         <v>0</v>
       </c>
@@ -2990,7 +3027,7 @@
       <c r="D24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -3004,22 +3041,21 @@
         <v>14</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="13">
         <f>SUMIF(Tabela1[SPRINT],"SPRINT2",Tabela1[TAM('#)])</f>
         <v>176</v>
       </c>
-      <c r="M24" s="11">
-        <f>M22-M23</f>
-        <v>143.33333333333337</v>
-      </c>
-      <c r="N24" s="12">
+      <c r="M24" s="13">
+        <v>148</v>
+      </c>
+      <c r="N24" s="11">
         <f>SUMIFS(Tabela1[TAM('#)],Tabela1[ESTADO],"FINALIZADO",Tabela1[SPRINT],"SPRINT2")</f>
         <v>176</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="13">
         <f>SUM(L24-N24)</f>
         <v>0</v>
       </c>
@@ -3037,7 +3073,7 @@
       <c r="D25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -3050,23 +3086,22 @@
       <c r="H25" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="13">
         <f>SUMIF(Tabela1[SPRINT],"SPRINT3",Tabela1[TAM('#)])</f>
         <v>81</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="13">
+        <v>117</v>
+      </c>
+      <c r="N25" s="11">
+        <v>81</v>
+      </c>
+      <c r="O25" s="13">
+        <f>SUM(L25-N25)</f>
         <v>0</v>
-      </c>
-      <c r="N25" s="12">
-        <f>SUMIFS(Tabela1[TAM('#)],Tabela1[ESTADO],"FINALIZADO",Tabela1[SPRINT],"SPRINT3")</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="11">
-        <f>SUM(L25-N25)</f>
-        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="30" customHeight="1">
@@ -3082,7 +3117,7 @@
       <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3094,6 +3129,19 @@
       </c>
       <c r="H26" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="21">
+        <v>0</v>
+      </c>
+      <c r="M26" s="20">
+        <v>0</v>
+      </c>
+      <c r="N26" s="21"/>
+      <c r="O26" s="20">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="30" customHeight="1">
@@ -3109,7 +3157,7 @@
       <c r="D27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3136,7 +3184,7 @@
       <c r="D28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3163,7 +3211,7 @@
       <c r="D29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3190,7 +3238,7 @@
       <c r="D30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -3217,7 +3265,7 @@
       <c r="D31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3244,7 +3292,7 @@
       <c r="D32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -3271,7 +3319,7 @@
       <c r="D33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3298,7 +3346,7 @@
       <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -3325,7 +3373,7 @@
       <c r="D35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="12">
         <f t="shared" ref="E35:E52" si="1">IF(D35="P",5,IF(D35="PP",3,IF(D35="M",8,IF(D35="G",13,IF(D35="GG",21,"")))))</f>
         <v>8</v>
       </c>
@@ -3352,7 +3400,7 @@
       <c r="D36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3379,7 +3427,7 @@
       <c r="D37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3406,7 +3454,7 @@
       <c r="D38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="12">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3433,7 +3481,7 @@
       <c r="D39" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="12">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -3460,7 +3508,7 @@
       <c r="D40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="12">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -3487,7 +3535,7 @@
       <c r="D41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3514,7 +3562,7 @@
       <c r="D42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3541,7 +3589,7 @@
       <c r="D43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="12">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -3578,7 +3626,7 @@
       <c r="G44" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="14" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3901,24 +3949,19 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AEC3BB-633E-407C-BF76-ED19E102FC3F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A729CFA7192B0F4AA60BE2DF65F4BC74" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="571acb434632999db5ee38a13a8eaef4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="517f1c296c3d1a438ed59838590dd0f3" ns3:_="">
     <xsd:import namespace="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
@@ -4068,10 +4111,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E306DC-4D82-4FE5-B96D-A09D99E18E75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBF2F96-8E40-4E5F-94E3-F7E55AE7689F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4093,19 +4163,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBF2F96-8E40-4E5F-94E3-F7E55AE7689F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E306DC-4D82-4FE5-B96D-A09D99E18E75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8497f9ae-9c71-438c-b553-1e6fe8b1acb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>